<commit_message>
Actualizar `streamlit_app.py` para incluir la función `mapeado_resultado_final` y ajustar la carga de archivos. Se modificó la lógica de rellenado de datos en `rellenar_datos_faltantes_con_PT` para manejar nuevos casos de valores en blanco. Además, se actualizaron las funciones de procesamiento de pólizas en `lectura_datos_origen.py`, `occident.py` y `producciontotal.py` para incluir nuevas columnas de datos. Se realizaron cambios en los archivos de caché correspondientes.
</commit_message>
<xml_diff>
--- a/tablas_origen/tablas_conversion_polizas.xlsx
+++ b/tablas_origen/tablas_conversion_polizas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daekka\Documents\Proyectos\Proyectos Diego\MBP_Evolution_NEXUS\Codigo JS\tablas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daekka\Documents\Proyectos\Proyectos Diego\MBP_streamlit\tablas_origen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8305307-EC31-4D46-A4AD-56E21156E3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6AF709-13AB-47B8-9464-9D30DC92BC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
   <si>
     <t>COSNOR</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>M_RENOVACION</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>F_NACIMIENTO</t>
   </si>
 </sst>
 </file>
@@ -277,7 +283,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +330,22 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -381,7 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -409,9 +431,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -533,8 +554,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B284A6B9-E02F-470D-A4CE-57846C9D7DF8}" name="tbl_polizas" displayName="tbl_polizas" ref="A1:F33" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
-  <autoFilter ref="A1:F33" xr:uid="{B284A6B9-E02F-470D-A4CE-57846C9D7DF8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B284A6B9-E02F-470D-A4CE-57846C9D7DF8}" name="tbl_polizas" displayName="tbl_polizas" ref="A1:F35" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
+  <autoFilter ref="A1:F35" xr:uid="{B284A6B9-E02F-470D-A4CE-57846C9D7DF8}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E16E29AE-9AD1-4497-B450-A370890DF018}" name="Columna" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{5181E023-1169-417E-9448-01501619A73F}" name="COSNOR" dataDxfId="3"/>
@@ -810,13 +831,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="20" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="22" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,304 +903,313 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>61</v>
-      </c>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>62</v>
+        <v>37</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>64</v>
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>65</v>
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>66</v>
+        <v>41</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>67</v>
+        <v>42</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>69</v>
+        <v>44</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>70</v>
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="F23" s="15"/>
+      <c r="A23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>26</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F33" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F8" xr:uid="{09271901-DD2A-4301-A7CF-314BF25DF502}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10" xr:uid="{09271901-DD2A-4301-A7CF-314BF25DF502}">
       <formula1>"AUTO,HOGAR,INTERNAUTO MOTO,VIDA,ACCIDENTES,DECESOS,DENTAL,COMERCIO,DRIVER,LEGAL,SPORT,BICI,GLOBAL,RC,PYME,RETIRADA CARNET,SEGURO VIAJE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13" xr:uid="{B9212E8A-C006-4E92-8450-AB6ACB9C8FE0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F15" xr:uid="{B9212E8A-C006-4E92-8450-AB6ACB9C8FE0}">
       <formula1>"ENVIADA,PENDIENTE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizar `lectura_datos_origen.py` para incluir la columna 'PRIMA_FRACCIONADA' en el mapeo de resultados y ajustar la lógica de cálculo de 'PRIMA_NETA' en `occident.py`. Se realizaron cambios en los archivos de caché y se actualizó el archivo de Excel `tablas_conversion_polizas.xlsx` para reflejar estas modificaciones.
</commit_message>
<xml_diff>
--- a/tablas_origen/tablas_conversion_polizas.xlsx
+++ b/tablas_origen/tablas_conversion_polizas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daekka\Documents\Proyectos\Proyectos Diego\MBP_streamlit\tablas_origen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6AF709-13AB-47B8-9464-9D30DC92BC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B06B882-00B8-4F35-9E34-D5CE55E4F41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t>COSNOR</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>F_NACIMIENTO</t>
+  </si>
+  <si>
+    <t>PRIMA_FRACCIONADA</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -435,6 +438,9 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -554,8 +560,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B284A6B9-E02F-470D-A4CE-57846C9D7DF8}" name="tbl_polizas" displayName="tbl_polizas" ref="A1:F35" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
-  <autoFilter ref="A1:F35" xr:uid="{B284A6B9-E02F-470D-A4CE-57846C9D7DF8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B284A6B9-E02F-470D-A4CE-57846C9D7DF8}" name="tbl_polizas" displayName="tbl_polizas" ref="A1:F36" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
+  <autoFilter ref="A1:F36" xr:uid="{B284A6B9-E02F-470D-A4CE-57846C9D7DF8}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E16E29AE-9AD1-4497-B450-A370890DF018}" name="Columna" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{5181E023-1169-417E-9448-01501619A73F}" name="COSNOR" dataDxfId="3"/>
@@ -831,18 +837,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="22" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="42.42578125" customWidth="1"/>
     <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
@@ -1156,44 +1162,53 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="F30" s="16"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F34" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>